<commit_message>
feature(db-compare) adjust excel format
</commit_message>
<xml_diff>
--- a/src/main/resources/compResult.xlsx
+++ b/src/main/resources/compResult.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\self_development\code\db-compare\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEB858F-683C-4F3D-9E4A-37AE604C4FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC3A272-DED4-4FEC-B850-A11DFC6EF4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="2244" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -110,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否可为NULL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>数据类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -243,6 +239,10 @@
   </si>
   <si>
     <t>{.tableCommentR}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nullable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -293,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -301,32 +301,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -334,7 +337,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,135 +631,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E699DE8F-F9C0-4132-A926-D5D096150173}">
   <dimension ref="A1:V326"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="17.34765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="5.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="1" customWidth="1"/>
     <col min="9" max="10" width="11.296875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="19.796875" style="6" customWidth="1"/>
+    <col min="11" max="12" width="19.796875" style="3" customWidth="1"/>
     <col min="13" max="18" width="11.5" style="1" customWidth="1"/>
     <col min="19" max="20" width="18.59765625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="19" style="6" customWidth="1"/>
+    <col min="21" max="22" width="19" style="3" customWidth="1"/>
     <col min="23" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="R1" s="6"/>
+      <c r="S1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9" t="s">
+      <c r="T1" s="6"/>
+      <c r="U1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="3" t="s">
+      <c r="V1" s="6"/>
+    </row>
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -759,1304 +771,1304 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
     </row>
     <row r="17" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
     </row>
     <row r="18" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
     </row>
     <row r="19" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
     </row>
     <row r="20" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
     </row>
     <row r="21" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
     </row>
     <row r="22" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
     </row>
     <row r="23" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
     </row>
     <row r="24" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S24" s="4"/>
+      <c r="S24" s="2"/>
     </row>
     <row r="25" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S25" s="4"/>
+      <c r="S25" s="2"/>
     </row>
     <row r="26" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S26" s="4"/>
+      <c r="S26" s="2"/>
     </row>
     <row r="27" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S27" s="4"/>
+      <c r="S27" s="2"/>
     </row>
     <row r="28" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S28" s="4"/>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S29" s="4"/>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
     </row>
     <row r="31" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
     </row>
     <row r="32" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
     </row>
     <row r="33" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
     </row>
     <row r="34" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
     </row>
     <row r="35" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
     </row>
     <row r="36" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
     </row>
     <row r="37" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T37" s="4"/>
+      <c r="T37" s="2"/>
     </row>
     <row r="38" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T38" s="4"/>
+      <c r="T38" s="2"/>
     </row>
     <row r="39" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T39" s="4"/>
+      <c r="T39" s="2"/>
     </row>
     <row r="40" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T40" s="4"/>
+      <c r="T40" s="2"/>
     </row>
     <row r="41" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
     </row>
     <row r="42" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
     </row>
     <row r="43" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
     </row>
     <row r="44" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T44" s="4"/>
+      <c r="T44" s="2"/>
     </row>
     <row r="45" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T45" s="4"/>
+      <c r="T45" s="2"/>
     </row>
     <row r="46" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
     </row>
     <row r="47" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
     </row>
     <row r="48" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
     </row>
     <row r="49" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T49" s="4"/>
+      <c r="T49" s="2"/>
     </row>
     <row r="50" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T50" s="4"/>
+      <c r="T50" s="2"/>
     </row>
     <row r="51" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
     </row>
     <row r="52" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
     </row>
     <row r="53" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
     </row>
     <row r="54" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
     </row>
     <row r="55" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
     </row>
     <row r="56" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
     </row>
     <row r="57" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
     </row>
     <row r="58" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
     </row>
     <row r="59" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
     </row>
     <row r="60" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
     </row>
     <row r="61" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
     </row>
     <row r="62" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
+      <c r="S62" s="2"/>
+      <c r="T62" s="2"/>
     </row>
     <row r="63" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
+      <c r="S63" s="2"/>
+      <c r="T63" s="2"/>
     </row>
     <row r="64" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
+      <c r="S64" s="2"/>
+      <c r="T64" s="2"/>
     </row>
     <row r="65" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
+      <c r="S65" s="2"/>
+      <c r="T65" s="2"/>
     </row>
     <row r="66" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
+      <c r="S66" s="2"/>
+      <c r="T66" s="2"/>
     </row>
     <row r="67" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
+      <c r="S67" s="2"/>
+      <c r="T67" s="2"/>
     </row>
     <row r="68" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
     </row>
     <row r="69" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S69" s="4"/>
-      <c r="T69" s="4"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
     </row>
     <row r="70" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
+      <c r="S70" s="2"/>
+      <c r="T70" s="2"/>
     </row>
     <row r="71" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S71" s="4"/>
-      <c r="T71" s="4"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
     </row>
     <row r="72" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T72" s="4"/>
+      <c r="T72" s="2"/>
     </row>
     <row r="73" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S73" s="4"/>
-      <c r="T73" s="4"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
     </row>
     <row r="74" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S74" s="4"/>
-      <c r="T74" s="4"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
     </row>
     <row r="75" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S75" s="4"/>
-      <c r="T75" s="4"/>
+      <c r="S75" s="2"/>
+      <c r="T75" s="2"/>
     </row>
     <row r="76" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S76" s="4"/>
-      <c r="T76" s="4"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
     </row>
     <row r="77" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S77" s="4"/>
-      <c r="T77" s="4"/>
+      <c r="S77" s="2"/>
+      <c r="T77" s="2"/>
     </row>
     <row r="78" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S78" s="4"/>
-      <c r="T78" s="4"/>
+      <c r="S78" s="2"/>
+      <c r="T78" s="2"/>
     </row>
     <row r="79" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S79" s="4"/>
-      <c r="T79" s="4"/>
+      <c r="S79" s="2"/>
+      <c r="T79" s="2"/>
     </row>
     <row r="80" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S80" s="4"/>
-      <c r="T80" s="4"/>
+      <c r="S80" s="2"/>
+      <c r="T80" s="2"/>
     </row>
     <row r="81" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
+      <c r="S81" s="2"/>
+      <c r="T81" s="2"/>
     </row>
     <row r="82" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S82" s="4"/>
-      <c r="T82" s="4"/>
+      <c r="S82" s="2"/>
+      <c r="T82" s="2"/>
     </row>
     <row r="83" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S83" s="4"/>
-      <c r="T83" s="4"/>
+      <c r="S83" s="2"/>
+      <c r="T83" s="2"/>
     </row>
     <row r="84" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S84" s="4"/>
-      <c r="T84" s="4"/>
+      <c r="S84" s="2"/>
+      <c r="T84" s="2"/>
     </row>
     <row r="85" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
+      <c r="S85" s="2"/>
+      <c r="T85" s="2"/>
     </row>
     <row r="86" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
+      <c r="S86" s="2"/>
+      <c r="T86" s="2"/>
     </row>
     <row r="87" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S87" s="4"/>
-      <c r="T87" s="4"/>
+      <c r="S87" s="2"/>
+      <c r="T87" s="2"/>
     </row>
     <row r="88" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S88" s="4"/>
-      <c r="T88" s="4"/>
+      <c r="S88" s="2"/>
+      <c r="T88" s="2"/>
     </row>
     <row r="89" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S89" s="4"/>
-      <c r="T89" s="4"/>
+      <c r="S89" s="2"/>
+      <c r="T89" s="2"/>
     </row>
     <row r="90" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S90" s="4"/>
-      <c r="T90" s="4"/>
+      <c r="S90" s="2"/>
+      <c r="T90" s="2"/>
     </row>
     <row r="91" spans="19:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="S91" s="4"/>
-      <c r="T91" s="4"/>
+      <c r="S91" s="2"/>
+      <c r="T91" s="2"/>
     </row>
     <row r="92" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
     </row>
     <row r="93" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S93" s="4"/>
-      <c r="T93" s="4"/>
+      <c r="S93" s="2"/>
+      <c r="T93" s="2"/>
     </row>
     <row r="94" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S94" s="4"/>
-      <c r="T94" s="4"/>
+      <c r="S94" s="2"/>
+      <c r="T94" s="2"/>
     </row>
     <row r="95" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S95" s="4"/>
-      <c r="T95" s="4"/>
+      <c r="S95" s="2"/>
+      <c r="T95" s="2"/>
     </row>
     <row r="96" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S96" s="4"/>
-      <c r="T96" s="4"/>
+      <c r="S96" s="2"/>
+      <c r="T96" s="2"/>
     </row>
     <row r="97" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S97" s="4"/>
-      <c r="T97" s="4"/>
+      <c r="S97" s="2"/>
+      <c r="T97" s="2"/>
     </row>
     <row r="98" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S98" s="4"/>
-      <c r="T98" s="4"/>
+      <c r="S98" s="2"/>
+      <c r="T98" s="2"/>
     </row>
     <row r="99" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S99" s="4"/>
-      <c r="T99" s="4"/>
+      <c r="S99" s="2"/>
+      <c r="T99" s="2"/>
     </row>
     <row r="100" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S100" s="4"/>
-      <c r="T100" s="4"/>
+      <c r="S100" s="2"/>
+      <c r="T100" s="2"/>
     </row>
     <row r="101" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
+      <c r="S101" s="2"/>
+      <c r="T101" s="2"/>
     </row>
     <row r="102" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T102" s="4"/>
+      <c r="T102" s="2"/>
     </row>
     <row r="103" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T103" s="4"/>
+      <c r="T103" s="2"/>
     </row>
     <row r="104" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T104" s="4"/>
+      <c r="T104" s="2"/>
     </row>
     <row r="105" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T105" s="4"/>
+      <c r="T105" s="2"/>
     </row>
     <row r="106" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T106" s="4"/>
+      <c r="T106" s="2"/>
     </row>
     <row r="107" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T107" s="4"/>
+      <c r="T107" s="2"/>
     </row>
     <row r="108" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T108" s="4"/>
+      <c r="T108" s="2"/>
     </row>
     <row r="109" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T109" s="4"/>
+      <c r="T109" s="2"/>
     </row>
     <row r="110" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T110" s="4"/>
+      <c r="T110" s="2"/>
     </row>
     <row r="111" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T111" s="4"/>
+      <c r="T111" s="2"/>
     </row>
     <row r="112" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T112" s="4"/>
+      <c r="T112" s="2"/>
     </row>
     <row r="113" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T113" s="4"/>
+      <c r="T113" s="2"/>
     </row>
     <row r="114" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T114" s="4"/>
+      <c r="T114" s="2"/>
     </row>
     <row r="115" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T115" s="4"/>
+      <c r="T115" s="2"/>
     </row>
     <row r="116" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S116" s="4"/>
-      <c r="T116" s="4"/>
+      <c r="S116" s="2"/>
+      <c r="T116" s="2"/>
     </row>
     <row r="117" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S117" s="4"/>
-      <c r="T117" s="4"/>
+      <c r="S117" s="2"/>
+      <c r="T117" s="2"/>
     </row>
     <row r="118" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S118" s="4"/>
-      <c r="T118" s="4"/>
+      <c r="S118" s="2"/>
+      <c r="T118" s="2"/>
     </row>
     <row r="119" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S119" s="4"/>
-      <c r="T119" s="4"/>
+      <c r="S119" s="2"/>
+      <c r="T119" s="2"/>
     </row>
     <row r="120" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S120" s="4"/>
-      <c r="T120" s="4"/>
+      <c r="S120" s="2"/>
+      <c r="T120" s="2"/>
     </row>
     <row r="121" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S121" s="4"/>
-      <c r="T121" s="4"/>
+      <c r="S121" s="2"/>
+      <c r="T121" s="2"/>
     </row>
     <row r="122" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T122" s="4"/>
+      <c r="T122" s="2"/>
     </row>
     <row r="123" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T123" s="4"/>
+      <c r="T123" s="2"/>
     </row>
     <row r="124" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T124" s="4"/>
+      <c r="T124" s="2"/>
     </row>
     <row r="125" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S125" s="4"/>
-      <c r="T125" s="4"/>
+      <c r="S125" s="2"/>
+      <c r="T125" s="2"/>
     </row>
     <row r="126" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S126" s="4"/>
-      <c r="T126" s="4"/>
+      <c r="S126" s="2"/>
+      <c r="T126" s="2"/>
     </row>
     <row r="127" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S127" s="4"/>
-      <c r="T127" s="4"/>
+      <c r="S127" s="2"/>
+      <c r="T127" s="2"/>
     </row>
     <row r="128" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S128" s="4"/>
-      <c r="T128" s="4"/>
+      <c r="S128" s="2"/>
+      <c r="T128" s="2"/>
     </row>
     <row r="129" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S129" s="4"/>
-      <c r="T129" s="4"/>
+      <c r="S129" s="2"/>
+      <c r="T129" s="2"/>
     </row>
     <row r="130" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S130" s="4"/>
-      <c r="T130" s="4"/>
+      <c r="S130" s="2"/>
+      <c r="T130" s="2"/>
     </row>
     <row r="131" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S131" s="4"/>
-      <c r="T131" s="4"/>
+      <c r="S131" s="2"/>
+      <c r="T131" s="2"/>
     </row>
     <row r="132" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
+      <c r="S132" s="2"/>
+      <c r="T132" s="2"/>
     </row>
     <row r="133" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S133" s="4"/>
-      <c r="T133" s="4"/>
+      <c r="S133" s="2"/>
+      <c r="T133" s="2"/>
     </row>
     <row r="134" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S134" s="4"/>
-      <c r="T134" s="4"/>
+      <c r="S134" s="2"/>
+      <c r="T134" s="2"/>
     </row>
     <row r="135" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S135" s="4"/>
-      <c r="T135" s="4"/>
+      <c r="S135" s="2"/>
+      <c r="T135" s="2"/>
     </row>
     <row r="136" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S136" s="4"/>
-      <c r="T136" s="4"/>
+      <c r="S136" s="2"/>
+      <c r="T136" s="2"/>
     </row>
     <row r="137" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S137" s="4"/>
-      <c r="T137" s="4"/>
+      <c r="S137" s="2"/>
+      <c r="T137" s="2"/>
     </row>
     <row r="138" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S138" s="4"/>
-      <c r="T138" s="4"/>
+      <c r="S138" s="2"/>
+      <c r="T138" s="2"/>
     </row>
     <row r="139" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
+      <c r="S139" s="2"/>
+      <c r="T139" s="2"/>
     </row>
     <row r="140" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S140" s="4"/>
-      <c r="T140" s="4"/>
+      <c r="S140" s="2"/>
+      <c r="T140" s="2"/>
     </row>
     <row r="141" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S141" s="4"/>
-      <c r="T141" s="4"/>
+      <c r="S141" s="2"/>
+      <c r="T141" s="2"/>
     </row>
     <row r="142" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S142" s="4"/>
-      <c r="T142" s="4"/>
+      <c r="S142" s="2"/>
+      <c r="T142" s="2"/>
     </row>
     <row r="143" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S143" s="4"/>
-      <c r="T143" s="4"/>
+      <c r="S143" s="2"/>
+      <c r="T143" s="2"/>
     </row>
     <row r="144" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S144" s="4"/>
-      <c r="T144" s="4"/>
+      <c r="S144" s="2"/>
+      <c r="T144" s="2"/>
     </row>
     <row r="145" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S145" s="4"/>
-      <c r="T145" s="4"/>
+      <c r="S145" s="2"/>
+      <c r="T145" s="2"/>
     </row>
     <row r="146" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S146" s="4"/>
-      <c r="T146" s="4"/>
+      <c r="S146" s="2"/>
+      <c r="T146" s="2"/>
     </row>
     <row r="147" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S147" s="4"/>
-      <c r="T147" s="4"/>
+      <c r="S147" s="2"/>
+      <c r="T147" s="2"/>
     </row>
     <row r="148" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S148" s="4"/>
-      <c r="T148" s="4"/>
+      <c r="S148" s="2"/>
+      <c r="T148" s="2"/>
     </row>
     <row r="149" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S149" s="4"/>
-      <c r="T149" s="4"/>
+      <c r="S149" s="2"/>
+      <c r="T149" s="2"/>
     </row>
     <row r="150" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S150" s="4"/>
-      <c r="T150" s="4"/>
+      <c r="S150" s="2"/>
+      <c r="T150" s="2"/>
     </row>
     <row r="151" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S151" s="4"/>
-      <c r="T151" s="4"/>
+      <c r="S151" s="2"/>
+      <c r="T151" s="2"/>
     </row>
     <row r="152" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S152" s="4"/>
-      <c r="T152" s="4"/>
+      <c r="S152" s="2"/>
+      <c r="T152" s="2"/>
     </row>
     <row r="153" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S153" s="4"/>
-      <c r="T153" s="4"/>
+      <c r="S153" s="2"/>
+      <c r="T153" s="2"/>
     </row>
     <row r="154" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S154" s="4"/>
-      <c r="T154" s="4"/>
+      <c r="S154" s="2"/>
+      <c r="T154" s="2"/>
     </row>
     <row r="155" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S155" s="4"/>
-      <c r="T155" s="4"/>
+      <c r="S155" s="2"/>
+      <c r="T155" s="2"/>
     </row>
     <row r="156" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S156" s="4"/>
-      <c r="T156" s="4"/>
+      <c r="S156" s="2"/>
+      <c r="T156" s="2"/>
     </row>
     <row r="157" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S157" s="4"/>
-      <c r="T157" s="4"/>
+      <c r="S157" s="2"/>
+      <c r="T157" s="2"/>
     </row>
     <row r="158" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S158" s="4"/>
-      <c r="T158" s="4"/>
+      <c r="S158" s="2"/>
+      <c r="T158" s="2"/>
     </row>
     <row r="159" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S159" s="4"/>
-      <c r="T159" s="4"/>
+      <c r="S159" s="2"/>
+      <c r="T159" s="2"/>
     </row>
     <row r="160" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S160" s="4"/>
-      <c r="T160" s="4"/>
+      <c r="S160" s="2"/>
+      <c r="T160" s="2"/>
     </row>
     <row r="161" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S161" s="4"/>
-      <c r="T161" s="4"/>
+      <c r="S161" s="2"/>
+      <c r="T161" s="2"/>
     </row>
     <row r="162" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S162" s="4"/>
-      <c r="T162" s="4"/>
+      <c r="S162" s="2"/>
+      <c r="T162" s="2"/>
     </row>
     <row r="163" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S163" s="4"/>
-      <c r="T163" s="4"/>
+      <c r="S163" s="2"/>
+      <c r="T163" s="2"/>
     </row>
     <row r="164" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S164" s="4"/>
-      <c r="T164" s="4"/>
+      <c r="S164" s="2"/>
+      <c r="T164" s="2"/>
     </row>
     <row r="165" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S165" s="4"/>
-      <c r="T165" s="4"/>
+      <c r="S165" s="2"/>
+      <c r="T165" s="2"/>
     </row>
     <row r="166" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T166" s="4"/>
+      <c r="T166" s="2"/>
     </row>
     <row r="167" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T167" s="4"/>
+      <c r="T167" s="2"/>
     </row>
     <row r="168" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S168" s="4"/>
-      <c r="T168" s="4"/>
+      <c r="S168" s="2"/>
+      <c r="T168" s="2"/>
     </row>
     <row r="169" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S169" s="4"/>
-      <c r="T169" s="4"/>
+      <c r="S169" s="2"/>
+      <c r="T169" s="2"/>
     </row>
     <row r="170" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S170" s="4"/>
-      <c r="T170" s="4"/>
+      <c r="S170" s="2"/>
+      <c r="T170" s="2"/>
     </row>
     <row r="171" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S171" s="4"/>
-      <c r="T171" s="4"/>
+      <c r="S171" s="2"/>
+      <c r="T171" s="2"/>
     </row>
     <row r="172" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S172" s="4"/>
-      <c r="T172" s="4"/>
+      <c r="S172" s="2"/>
+      <c r="T172" s="2"/>
     </row>
     <row r="173" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S173" s="4"/>
-      <c r="T173" s="4"/>
+      <c r="S173" s="2"/>
+      <c r="T173" s="2"/>
     </row>
     <row r="174" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S174" s="4"/>
-      <c r="T174" s="4"/>
+      <c r="S174" s="2"/>
+      <c r="T174" s="2"/>
     </row>
     <row r="175" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S175" s="4"/>
-      <c r="T175" s="4"/>
+      <c r="S175" s="2"/>
+      <c r="T175" s="2"/>
     </row>
     <row r="176" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S176" s="4"/>
-      <c r="T176" s="4"/>
+      <c r="S176" s="2"/>
+      <c r="T176" s="2"/>
     </row>
     <row r="177" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S177" s="4"/>
-      <c r="T177" s="4"/>
+      <c r="S177" s="2"/>
+      <c r="T177" s="2"/>
     </row>
     <row r="178" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S178" s="4"/>
-      <c r="T178" s="4"/>
+      <c r="S178" s="2"/>
+      <c r="T178" s="2"/>
     </row>
     <row r="179" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S179" s="4"/>
-      <c r="T179" s="4"/>
+      <c r="S179" s="2"/>
+      <c r="T179" s="2"/>
     </row>
     <row r="180" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S180" s="4"/>
-      <c r="T180" s="4"/>
+      <c r="S180" s="2"/>
+      <c r="T180" s="2"/>
     </row>
     <row r="181" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S181" s="4"/>
-      <c r="T181" s="4"/>
+      <c r="S181" s="2"/>
+      <c r="T181" s="2"/>
     </row>
     <row r="182" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S182" s="4"/>
-      <c r="T182" s="4"/>
+      <c r="S182" s="2"/>
+      <c r="T182" s="2"/>
     </row>
     <row r="183" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S183" s="4"/>
-      <c r="T183" s="4"/>
+      <c r="S183" s="2"/>
+      <c r="T183" s="2"/>
     </row>
     <row r="184" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S184" s="4"/>
-      <c r="T184" s="4"/>
+      <c r="S184" s="2"/>
+      <c r="T184" s="2"/>
     </row>
     <row r="185" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S185" s="4"/>
-      <c r="T185" s="4"/>
+      <c r="S185" s="2"/>
+      <c r="T185" s="2"/>
     </row>
     <row r="186" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S186" s="4"/>
-      <c r="T186" s="4"/>
+      <c r="S186" s="2"/>
+      <c r="T186" s="2"/>
     </row>
     <row r="187" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S187" s="4"/>
-      <c r="T187" s="4"/>
+      <c r="S187" s="2"/>
+      <c r="T187" s="2"/>
     </row>
     <row r="188" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S188" s="4"/>
-      <c r="T188" s="4"/>
+      <c r="S188" s="2"/>
+      <c r="T188" s="2"/>
     </row>
     <row r="189" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S189" s="4"/>
-      <c r="T189" s="4"/>
+      <c r="S189" s="2"/>
+      <c r="T189" s="2"/>
     </row>
     <row r="190" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S190" s="4"/>
-      <c r="T190" s="4"/>
+      <c r="S190" s="2"/>
+      <c r="T190" s="2"/>
     </row>
     <row r="191" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S191" s="4"/>
-      <c r="T191" s="4"/>
+      <c r="S191" s="2"/>
+      <c r="T191" s="2"/>
     </row>
     <row r="192" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S192" s="4"/>
-      <c r="T192" s="4"/>
+      <c r="S192" s="2"/>
+      <c r="T192" s="2"/>
     </row>
     <row r="193" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S193" s="4"/>
-      <c r="T193" s="4"/>
+      <c r="S193" s="2"/>
+      <c r="T193" s="2"/>
     </row>
     <row r="194" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S194" s="4"/>
-      <c r="T194" s="4"/>
+      <c r="S194" s="2"/>
+      <c r="T194" s="2"/>
     </row>
     <row r="195" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S195" s="4"/>
-      <c r="T195" s="4"/>
+      <c r="S195" s="2"/>
+      <c r="T195" s="2"/>
     </row>
     <row r="196" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S196" s="4"/>
-      <c r="T196" s="4"/>
+      <c r="S196" s="2"/>
+      <c r="T196" s="2"/>
     </row>
     <row r="197" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S197" s="4"/>
-      <c r="T197" s="4"/>
+      <c r="S197" s="2"/>
+      <c r="T197" s="2"/>
     </row>
     <row r="198" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S198" s="4"/>
-      <c r="T198" s="4"/>
+      <c r="S198" s="2"/>
+      <c r="T198" s="2"/>
     </row>
     <row r="199" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S199" s="4"/>
-      <c r="T199" s="4"/>
+      <c r="S199" s="2"/>
+      <c r="T199" s="2"/>
     </row>
     <row r="200" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S200" s="4"/>
-      <c r="T200" s="4"/>
+      <c r="S200" s="2"/>
+      <c r="T200" s="2"/>
     </row>
     <row r="201" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S201" s="4"/>
-      <c r="T201" s="4"/>
+      <c r="S201" s="2"/>
+      <c r="T201" s="2"/>
     </row>
     <row r="202" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S202" s="4"/>
-      <c r="T202" s="4"/>
+      <c r="S202" s="2"/>
+      <c r="T202" s="2"/>
     </row>
     <row r="203" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T203" s="4"/>
+      <c r="T203" s="2"/>
     </row>
     <row r="204" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S204" s="4"/>
-      <c r="T204" s="4"/>
+      <c r="S204" s="2"/>
+      <c r="T204" s="2"/>
     </row>
     <row r="205" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T205" s="4"/>
+      <c r="T205" s="2"/>
     </row>
     <row r="206" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S206" s="4"/>
-      <c r="T206" s="4"/>
+      <c r="S206" s="2"/>
+      <c r="T206" s="2"/>
     </row>
     <row r="207" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T207" s="4"/>
+      <c r="T207" s="2"/>
     </row>
     <row r="208" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S208" s="4"/>
-      <c r="T208" s="4"/>
+      <c r="S208" s="2"/>
+      <c r="T208" s="2"/>
     </row>
     <row r="209" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S209" s="4"/>
-      <c r="T209" s="4"/>
+      <c r="S209" s="2"/>
+      <c r="T209" s="2"/>
     </row>
     <row r="210" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S210" s="4"/>
-      <c r="T210" s="4"/>
+      <c r="S210" s="2"/>
+      <c r="T210" s="2"/>
     </row>
     <row r="211" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S211" s="4"/>
-      <c r="T211" s="4"/>
+      <c r="S211" s="2"/>
+      <c r="T211" s="2"/>
     </row>
     <row r="212" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S212" s="4"/>
-      <c r="T212" s="4"/>
+      <c r="S212" s="2"/>
+      <c r="T212" s="2"/>
     </row>
     <row r="213" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S213" s="4"/>
-      <c r="T213" s="4"/>
+      <c r="S213" s="2"/>
+      <c r="T213" s="2"/>
     </row>
     <row r="214" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S214" s="4"/>
-      <c r="T214" s="4"/>
+      <c r="S214" s="2"/>
+      <c r="T214" s="2"/>
     </row>
     <row r="215" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S215" s="4"/>
-      <c r="T215" s="4"/>
+      <c r="S215" s="2"/>
+      <c r="T215" s="2"/>
     </row>
     <row r="216" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S216" s="4"/>
-      <c r="T216" s="4"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="2"/>
     </row>
     <row r="217" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S217" s="4"/>
-      <c r="T217" s="4"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="2"/>
     </row>
     <row r="218" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S218" s="4"/>
-      <c r="T218" s="4"/>
+      <c r="S218" s="2"/>
+      <c r="T218" s="2"/>
     </row>
     <row r="219" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S219" s="4"/>
-      <c r="T219" s="4"/>
+      <c r="S219" s="2"/>
+      <c r="T219" s="2"/>
     </row>
     <row r="220" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S220" s="4"/>
-      <c r="T220" s="4"/>
+      <c r="S220" s="2"/>
+      <c r="T220" s="2"/>
     </row>
     <row r="221" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S221" s="4"/>
-      <c r="T221" s="4"/>
+      <c r="S221" s="2"/>
+      <c r="T221" s="2"/>
     </row>
     <row r="222" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T222" s="4"/>
+      <c r="T222" s="2"/>
     </row>
     <row r="223" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T223" s="4"/>
+      <c r="T223" s="2"/>
     </row>
     <row r="224" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T224" s="4"/>
+      <c r="T224" s="2"/>
     </row>
     <row r="225" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S225" s="4"/>
-      <c r="T225" s="4"/>
+      <c r="S225" s="2"/>
+      <c r="T225" s="2"/>
     </row>
     <row r="226" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S226" s="4"/>
-      <c r="T226" s="4"/>
+      <c r="S226" s="2"/>
+      <c r="T226" s="2"/>
     </row>
     <row r="227" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S227" s="4"/>
-      <c r="T227" s="4"/>
+      <c r="S227" s="2"/>
+      <c r="T227" s="2"/>
     </row>
     <row r="228" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S228" s="4"/>
-      <c r="T228" s="4"/>
+      <c r="S228" s="2"/>
+      <c r="T228" s="2"/>
     </row>
     <row r="229" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S229" s="4"/>
-      <c r="T229" s="4"/>
+      <c r="S229" s="2"/>
+      <c r="T229" s="2"/>
     </row>
     <row r="230" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S230" s="4"/>
-      <c r="T230" s="4"/>
+      <c r="S230" s="2"/>
+      <c r="T230" s="2"/>
     </row>
     <row r="231" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S231" s="4"/>
-      <c r="T231" s="4"/>
+      <c r="S231" s="2"/>
+      <c r="T231" s="2"/>
     </row>
     <row r="232" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S232" s="4"/>
-      <c r="T232" s="4"/>
+      <c r="S232" s="2"/>
+      <c r="T232" s="2"/>
     </row>
     <row r="233" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S233" s="4"/>
-      <c r="T233" s="4"/>
+      <c r="S233" s="2"/>
+      <c r="T233" s="2"/>
     </row>
     <row r="234" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S234" s="4"/>
-      <c r="T234" s="4"/>
+      <c r="S234" s="2"/>
+      <c r="T234" s="2"/>
     </row>
     <row r="235" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S235" s="4"/>
-      <c r="T235" s="4"/>
+      <c r="S235" s="2"/>
+      <c r="T235" s="2"/>
     </row>
     <row r="236" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S236" s="4"/>
-      <c r="T236" s="4"/>
+      <c r="S236" s="2"/>
+      <c r="T236" s="2"/>
     </row>
     <row r="237" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S237" s="4"/>
-      <c r="T237" s="4"/>
+      <c r="S237" s="2"/>
+      <c r="T237" s="2"/>
     </row>
     <row r="238" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S238" s="4"/>
-      <c r="T238" s="4"/>
+      <c r="S238" s="2"/>
+      <c r="T238" s="2"/>
     </row>
     <row r="239" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S239" s="4"/>
-      <c r="T239" s="4"/>
+      <c r="S239" s="2"/>
+      <c r="T239" s="2"/>
     </row>
     <row r="240" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S240" s="4"/>
+      <c r="S240" s="2"/>
     </row>
     <row r="241" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S241" s="4"/>
-      <c r="T241" s="4"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="2"/>
     </row>
     <row r="242" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S242" s="4"/>
-      <c r="T242" s="4"/>
+      <c r="S242" s="2"/>
+      <c r="T242" s="2"/>
     </row>
     <row r="243" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S243" s="4"/>
-      <c r="T243" s="4"/>
+      <c r="S243" s="2"/>
+      <c r="T243" s="2"/>
     </row>
     <row r="244" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S244" s="4"/>
-      <c r="T244" s="4"/>
+      <c r="S244" s="2"/>
+      <c r="T244" s="2"/>
     </row>
     <row r="245" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S245" s="4"/>
-      <c r="T245" s="4"/>
+      <c r="S245" s="2"/>
+      <c r="T245" s="2"/>
     </row>
     <row r="246" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S246" s="4"/>
-      <c r="T246" s="4"/>
+      <c r="S246" s="2"/>
+      <c r="T246" s="2"/>
     </row>
     <row r="247" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S247" s="4"/>
-      <c r="T247" s="4"/>
+      <c r="S247" s="2"/>
+      <c r="T247" s="2"/>
     </row>
     <row r="248" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T248" s="4"/>
+      <c r="T248" s="2"/>
     </row>
     <row r="249" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S249" s="4"/>
-      <c r="T249" s="4"/>
+      <c r="S249" s="2"/>
+      <c r="T249" s="2"/>
     </row>
     <row r="250" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T250" s="4"/>
+      <c r="T250" s="2"/>
     </row>
     <row r="251" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S251" s="4"/>
-      <c r="T251" s="4"/>
+      <c r="S251" s="2"/>
+      <c r="T251" s="2"/>
     </row>
     <row r="252" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S252" s="4"/>
-      <c r="T252" s="4"/>
+      <c r="S252" s="2"/>
+      <c r="T252" s="2"/>
     </row>
     <row r="253" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T253" s="4"/>
+      <c r="T253" s="2"/>
     </row>
     <row r="254" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S254" s="4"/>
-      <c r="T254" s="4"/>
+      <c r="S254" s="2"/>
+      <c r="T254" s="2"/>
     </row>
     <row r="255" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S255" s="4"/>
-      <c r="T255" s="4"/>
+      <c r="S255" s="2"/>
+      <c r="T255" s="2"/>
     </row>
     <row r="256" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S256" s="4"/>
-      <c r="T256" s="4"/>
+      <c r="S256" s="2"/>
+      <c r="T256" s="2"/>
     </row>
     <row r="257" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S257" s="4"/>
-      <c r="T257" s="4"/>
+      <c r="S257" s="2"/>
+      <c r="T257" s="2"/>
     </row>
     <row r="258" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S258" s="4"/>
-      <c r="T258" s="4"/>
+      <c r="S258" s="2"/>
+      <c r="T258" s="2"/>
     </row>
     <row r="259" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S259" s="4"/>
-      <c r="T259" s="4"/>
+      <c r="S259" s="2"/>
+      <c r="T259" s="2"/>
     </row>
     <row r="260" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S260" s="4"/>
-      <c r="T260" s="4"/>
+      <c r="S260" s="2"/>
+      <c r="T260" s="2"/>
     </row>
     <row r="261" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S261" s="4"/>
-      <c r="T261" s="4"/>
+      <c r="S261" s="2"/>
+      <c r="T261" s="2"/>
     </row>
     <row r="262" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S262" s="4"/>
-      <c r="T262" s="4"/>
+      <c r="S262" s="2"/>
+      <c r="T262" s="2"/>
     </row>
     <row r="263" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S263" s="4"/>
-      <c r="T263" s="4"/>
+      <c r="S263" s="2"/>
+      <c r="T263" s="2"/>
     </row>
     <row r="264" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S264" s="4"/>
-      <c r="T264" s="4"/>
+      <c r="S264" s="2"/>
+      <c r="T264" s="2"/>
     </row>
     <row r="265" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S265" s="4"/>
-      <c r="T265" s="4"/>
+      <c r="S265" s="2"/>
+      <c r="T265" s="2"/>
     </row>
     <row r="266" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S266" s="4"/>
-      <c r="T266" s="4"/>
+      <c r="S266" s="2"/>
+      <c r="T266" s="2"/>
     </row>
     <row r="267" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S267" s="4"/>
-      <c r="T267" s="4"/>
+      <c r="S267" s="2"/>
+      <c r="T267" s="2"/>
     </row>
     <row r="268" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T268" s="4"/>
+      <c r="T268" s="2"/>
     </row>
     <row r="269" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S269" s="4"/>
-      <c r="T269" s="4"/>
+      <c r="S269" s="2"/>
+      <c r="T269" s="2"/>
     </row>
     <row r="270" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S270" s="4"/>
-      <c r="T270" s="4"/>
+      <c r="S270" s="2"/>
+      <c r="T270" s="2"/>
     </row>
     <row r="271" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S271" s="4"/>
-      <c r="T271" s="4"/>
+      <c r="S271" s="2"/>
+      <c r="T271" s="2"/>
     </row>
     <row r="272" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S272" s="4"/>
-      <c r="T272" s="4"/>
+      <c r="S272" s="2"/>
+      <c r="T272" s="2"/>
     </row>
     <row r="273" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S273" s="4"/>
-      <c r="T273" s="4"/>
+      <c r="S273" s="2"/>
+      <c r="T273" s="2"/>
     </row>
     <row r="274" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S274" s="4"/>
-      <c r="T274" s="4"/>
+      <c r="S274" s="2"/>
+      <c r="T274" s="2"/>
     </row>
     <row r="275" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T275" s="4"/>
+      <c r="T275" s="2"/>
     </row>
     <row r="276" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S276" s="4"/>
-      <c r="T276" s="4"/>
+      <c r="S276" s="2"/>
+      <c r="T276" s="2"/>
     </row>
     <row r="277" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S277" s="4"/>
-      <c r="T277" s="4"/>
+      <c r="S277" s="2"/>
+      <c r="T277" s="2"/>
     </row>
     <row r="278" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S278" s="4"/>
-      <c r="T278" s="4"/>
+      <c r="S278" s="2"/>
+      <c r="T278" s="2"/>
     </row>
     <row r="279" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S279" s="4"/>
-      <c r="T279" s="4"/>
+      <c r="S279" s="2"/>
+      <c r="T279" s="2"/>
     </row>
     <row r="280" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S280" s="4"/>
-      <c r="T280" s="4"/>
+      <c r="S280" s="2"/>
+      <c r="T280" s="2"/>
     </row>
     <row r="281" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S281" s="4"/>
-      <c r="T281" s="4"/>
+      <c r="S281" s="2"/>
+      <c r="T281" s="2"/>
     </row>
     <row r="282" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S282" s="4"/>
-      <c r="T282" s="4"/>
+      <c r="S282" s="2"/>
+      <c r="T282" s="2"/>
     </row>
     <row r="283" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S283" s="4"/>
-      <c r="T283" s="4"/>
+      <c r="S283" s="2"/>
+      <c r="T283" s="2"/>
     </row>
     <row r="284" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T284" s="4"/>
+      <c r="T284" s="2"/>
     </row>
     <row r="285" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S285" s="4"/>
-      <c r="T285" s="4"/>
+      <c r="S285" s="2"/>
+      <c r="T285" s="2"/>
     </row>
     <row r="286" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S286" s="4"/>
-      <c r="T286" s="4"/>
+      <c r="S286" s="2"/>
+      <c r="T286" s="2"/>
     </row>
     <row r="287" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S287" s="4"/>
-      <c r="T287" s="4"/>
+      <c r="S287" s="2"/>
+      <c r="T287" s="2"/>
     </row>
     <row r="288" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S288" s="4"/>
-      <c r="T288" s="4"/>
+      <c r="S288" s="2"/>
+      <c r="T288" s="2"/>
     </row>
     <row r="289" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T289" s="4"/>
+      <c r="T289" s="2"/>
     </row>
     <row r="290" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T290" s="4"/>
+      <c r="T290" s="2"/>
     </row>
     <row r="291" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T291" s="4"/>
+      <c r="T291" s="2"/>
     </row>
     <row r="292" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T292" s="4"/>
+      <c r="T292" s="2"/>
     </row>
     <row r="293" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S293" s="4"/>
-      <c r="T293" s="4"/>
+      <c r="S293" s="2"/>
+      <c r="T293" s="2"/>
     </row>
     <row r="294" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S294" s="4"/>
-      <c r="T294" s="4"/>
+      <c r="S294" s="2"/>
+      <c r="T294" s="2"/>
     </row>
     <row r="295" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S295" s="4"/>
-      <c r="T295" s="4"/>
+      <c r="S295" s="2"/>
+      <c r="T295" s="2"/>
     </row>
     <row r="296" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S296" s="4"/>
-      <c r="T296" s="4"/>
+      <c r="S296" s="2"/>
+      <c r="T296" s="2"/>
     </row>
     <row r="297" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S297" s="4"/>
-      <c r="T297" s="4"/>
+      <c r="S297" s="2"/>
+      <c r="T297" s="2"/>
     </row>
     <row r="298" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S298" s="4"/>
-      <c r="T298" s="4"/>
+      <c r="S298" s="2"/>
+      <c r="T298" s="2"/>
     </row>
     <row r="299" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S299" s="4"/>
-      <c r="T299" s="4"/>
+      <c r="S299" s="2"/>
+      <c r="T299" s="2"/>
     </row>
     <row r="300" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S300" s="4"/>
-      <c r="T300" s="4"/>
+      <c r="S300" s="2"/>
+      <c r="T300" s="2"/>
     </row>
     <row r="301" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S301" s="4"/>
-      <c r="T301" s="4"/>
+      <c r="S301" s="2"/>
+      <c r="T301" s="2"/>
     </row>
     <row r="302" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S302" s="4"/>
-      <c r="T302" s="4"/>
+      <c r="S302" s="2"/>
+      <c r="T302" s="2"/>
     </row>
     <row r="303" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S303" s="4"/>
-      <c r="T303" s="4"/>
+      <c r="S303" s="2"/>
+      <c r="T303" s="2"/>
     </row>
     <row r="304" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S304" s="4"/>
-      <c r="T304" s="4"/>
+      <c r="S304" s="2"/>
+      <c r="T304" s="2"/>
     </row>
     <row r="305" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S305" s="4"/>
-      <c r="T305" s="4"/>
+      <c r="S305" s="2"/>
+      <c r="T305" s="2"/>
     </row>
     <row r="306" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S306" s="4"/>
-      <c r="T306" s="4"/>
+      <c r="S306" s="2"/>
+      <c r="T306" s="2"/>
     </row>
     <row r="307" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S307" s="4"/>
-      <c r="T307" s="4"/>
+      <c r="S307" s="2"/>
+      <c r="T307" s="2"/>
     </row>
     <row r="308" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S308" s="4"/>
-      <c r="T308" s="4"/>
+      <c r="S308" s="2"/>
+      <c r="T308" s="2"/>
     </row>
     <row r="309" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S309" s="4"/>
-      <c r="T309" s="4"/>
+      <c r="S309" s="2"/>
+      <c r="T309" s="2"/>
     </row>
     <row r="310" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S310" s="4"/>
-      <c r="T310" s="4"/>
+      <c r="S310" s="2"/>
+      <c r="T310" s="2"/>
     </row>
     <row r="311" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S311" s="4"/>
+      <c r="S311" s="2"/>
     </row>
     <row r="312" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S312" s="4"/>
-      <c r="T312" s="4"/>
+      <c r="S312" s="2"/>
+      <c r="T312" s="2"/>
     </row>
     <row r="313" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S313" s="4"/>
-      <c r="T313" s="4"/>
+      <c r="S313" s="2"/>
+      <c r="T313" s="2"/>
     </row>
     <row r="314" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S314" s="4"/>
-      <c r="T314" s="4"/>
+      <c r="S314" s="2"/>
+      <c r="T314" s="2"/>
     </row>
     <row r="315" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S315" s="4"/>
-      <c r="T315" s="4"/>
+      <c r="S315" s="2"/>
+      <c r="T315" s="2"/>
     </row>
     <row r="316" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S316" s="4"/>
-      <c r="T316" s="4"/>
+      <c r="S316" s="2"/>
+      <c r="T316" s="2"/>
     </row>
     <row r="317" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S317" s="4"/>
-      <c r="T317" s="4"/>
+      <c r="S317" s="2"/>
+      <c r="T317" s="2"/>
     </row>
     <row r="318" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S318" s="4"/>
-      <c r="T318" s="4"/>
+      <c r="S318" s="2"/>
+      <c r="T318" s="2"/>
     </row>
     <row r="319" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="T319" s="4"/>
+      <c r="T319" s="2"/>
     </row>
     <row r="320" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S320" s="4"/>
-      <c r="T320" s="4"/>
+      <c r="S320" s="2"/>
+      <c r="T320" s="2"/>
     </row>
     <row r="321" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S321" s="4"/>
-      <c r="T321" s="4"/>
+      <c r="S321" s="2"/>
+      <c r="T321" s="2"/>
     </row>
     <row r="322" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S322" s="4"/>
-      <c r="T322" s="4"/>
+      <c r="S322" s="2"/>
+      <c r="T322" s="2"/>
     </row>
     <row r="323" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S323" s="4"/>
-      <c r="T323" s="4"/>
+      <c r="S323" s="2"/>
+      <c r="T323" s="2"/>
     </row>
     <row r="324" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S324" s="4"/>
-      <c r="T324" s="4"/>
+      <c r="S324" s="2"/>
+      <c r="T324" s="2"/>
     </row>
     <row r="325" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S325" s="4"/>
-      <c r="T325" s="4"/>
+      <c r="S325" s="2"/>
+      <c r="T325" s="2"/>
     </row>
     <row r="326" spans="19:20" x14ac:dyDescent="0.5">
-      <c r="S326" s="4"/>
-      <c r="T326" s="4"/>
+      <c r="S326" s="2"/>
+      <c r="T326" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:H95" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -2084,9 +2096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -2094,78 +2106,78 @@
     <col min="1" max="1" width="17.34765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.94921875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="5.94921875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="7" width="18.546875" style="1" customWidth="1"/>
     <col min="8" max="9" width="6.34765625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.19921875" style="8" customWidth="1"/>
+    <col min="12" max="13" width="20.19921875" style="4" customWidth="1"/>
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="3" t="s">
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2180,34 +2192,34 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="90" ht="14.4" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
feature(db-compare) modify excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/compResult.xlsx
+++ b/src/main/resources/compResult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\self_development\code\db-compare\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC3A272-DED4-4FEC-B850-A11DFC6EF4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A32A9B-4B54-4540-9A09-4895665E3571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -341,10 +341,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -633,7 +633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -644,7 +644,7 @@
     <col min="5" max="6" width="10.59765625" style="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1" customWidth="1"/>
     <col min="9" max="10" width="11.296875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="19.796875" style="3" customWidth="1"/>
+    <col min="11" max="12" width="19.796875" style="4" customWidth="1"/>
     <col min="13" max="18" width="11.5" style="1" customWidth="1"/>
     <col min="19" max="20" width="18.59765625" style="1" customWidth="1"/>
     <col min="21" max="22" width="19" style="3" customWidth="1"/>
@@ -652,78 +652,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6" t="s">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6" t="s">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="6"/>
+      <c r="V1" s="8"/>
     </row>
     <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -732,34 +732,34 @@
       <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -794,10 +794,10 @@
       <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -2096,9 +2096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -2116,68 +2116,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>